<commit_message>
Atualizando status do requisito Objetivo do projeto no BackLog
</commit_message>
<xml_diff>
--- a/docs/Backlog.xlsx
+++ b/docs/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>Status</t>
   </si>
@@ -944,7 +944,7 @@
     </row>
     <row r="14" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Apagando página Sobre Mim
</commit_message>
<xml_diff>
--- a/docs/Backlog.xlsx
+++ b/docs/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="64">
   <si>
     <t>Status</t>
   </si>
@@ -101,16 +101,10 @@
     <t>FAZER</t>
   </si>
   <si>
-    <t>Colocar conteúdo real na página Sobre mim</t>
-  </si>
-  <si>
     <t>Colocar conteúdo na Home</t>
   </si>
   <si>
     <t>Colocar conteúdo em Personagens</t>
-  </si>
-  <si>
-    <t>Colocar conteúdo na Sobre mim</t>
   </si>
   <si>
     <t>Validação na pagina de cadastro</t>
@@ -657,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I27"/>
+  <dimension ref="B2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +737,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>10</v>
@@ -832,7 +826,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>22</v>
@@ -855,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>23</v>
@@ -873,55 +867,55 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="12">
+        <v>5</v>
+      </c>
+      <c r="H11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="12">
-        <v>3</v>
-      </c>
-      <c r="H11" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="9">
+        <v>8</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="9">
-        <v>5</v>
-      </c>
-      <c r="H12" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
-        <v>31</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>33</v>
@@ -942,15 +936,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>10</v>
@@ -965,38 +959,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="12" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="E15" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="12">
+        <v>13</v>
+      </c>
+      <c r="H15" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="12">
-        <v>8</v>
-      </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>10</v>
@@ -1005,27 +999,27 @@
         <v>41</v>
       </c>
       <c r="G16" s="9">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="H16" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="E17" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G17" s="12">
         <v>21</v>
@@ -1034,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>7</v>
       </c>
@@ -1048,39 +1042,39 @@
         <v>10</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G18" s="9">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="H18" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G19" s="12">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H19" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>7</v>
       </c>
@@ -1103,9 +1097,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>52</v>
@@ -1114,21 +1108,21 @@
         <v>53</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="G21" s="12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H21" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>54</v>
@@ -1137,19 +1131,19 @@
         <v>55</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G22" s="9">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H22" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="12" t="s">
         <v>7</v>
       </c>
@@ -1163,16 +1157,16 @@
         <v>10</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="G23" s="12">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H23" s="12">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>7</v>
       </c>
@@ -1186,18 +1180,18 @@
         <v>10</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="G24" s="9">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="H24" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>60</v>
@@ -1206,19 +1200,19 @@
         <v>61</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="G25" s="12">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="H25" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="28.5" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>24</v>
       </c>
@@ -1229,38 +1223,15 @@
         <v>63</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G26" s="9">
         <v>5</v>
       </c>
       <c r="H26" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27" s="12">
-        <v>5</v>
-      </c>
-      <c r="H27" s="12">
         <v>1</v>
       </c>
     </row>

</xml_diff>